<commit_message>
Command-line interface uses **kwargs. Linking checks done in one place.
</commit_message>
<xml_diff>
--- a/qtools2/test/forms/child_form.xlsx
+++ b/qtools2/test/forms/child_form.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="26819"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="26929"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="25000" yWindow="6400" windowWidth="25600" windowHeight="14240" tabRatio="500"/>
+    <workbookView xWindow="25000" yWindow="6400" windowWidth="25600" windowHeight="14240" tabRatio="500" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="survey" sheetId="1" r:id="rId1"/>
@@ -98,9 +98,6 @@
     <t>child_form_id</t>
   </si>
   <si>
-    <t>Child Form 1</t>
-  </si>
-  <si>
     <t>xml_root</t>
   </si>
   <si>
@@ -129,6 +126,9 @@
   </si>
   <si>
     <t>yes</t>
+  </si>
+  <si>
+    <t>Child Form V</t>
   </si>
 </sst>
 </file>
@@ -523,7 +523,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G8"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="G9" sqref="G9"/>
     </sheetView>
   </sheetViews>
@@ -547,13 +547,13 @@
         <v>9</v>
       </c>
       <c r="E1" t="s">
+        <v>31</v>
+      </c>
+      <c r="F1" t="s">
         <v>32</v>
       </c>
-      <c r="F1" t="s">
-        <v>33</v>
-      </c>
       <c r="G1" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="2" spans="1:7">
@@ -610,24 +610,24 @@
     </row>
     <row r="7" spans="1:7">
       <c r="A7" t="s">
+        <v>27</v>
+      </c>
+      <c r="B7" t="s">
         <v>28</v>
-      </c>
-      <c r="B7" t="s">
-        <v>29</v>
       </c>
     </row>
     <row r="8" spans="1:7">
       <c r="A8" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B8" t="s">
+        <v>33</v>
+      </c>
+      <c r="F8" t="s">
+        <v>30</v>
+      </c>
+      <c r="G8" t="s">
         <v>34</v>
-      </c>
-      <c r="F8" t="s">
-        <v>31</v>
-      </c>
-      <c r="G8" t="s">
-        <v>35</v>
       </c>
     </row>
   </sheetData>
@@ -698,8 +698,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C2"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C3" sqref="C3"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -715,18 +715,18 @@
         <v>22</v>
       </c>
       <c r="C1" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
     <row r="2" spans="1:3">
       <c r="A2" t="s">
-        <v>25</v>
+        <v>35</v>
       </c>
       <c r="B2" t="s">
         <v>24</v>
       </c>
       <c r="C2" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
   </sheetData>

</xml_diff>